<commit_message>
Begin gemaakt aan de eerste kamer
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08cc52190196310d/Documenten/TBA/Non-Code Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7916A1DC-09DC-4251-B336-81ECA4145E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4342101-CA4A-40EE-9A93-908F2F873755}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{7916A1DC-09DC-4251-B336-81ECA4145E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C8BCE8-4BF3-4970-9294-8A0ADC49239E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Eerste 6 locaties bedacht en en basis van locaties uitgedacht</t>
+  </si>
+  <si>
+    <t>Nog 3 locaties toegevoegd met wat sublocaties in die locaties</t>
+  </si>
+  <si>
+    <t>Laatste voorlogie locatie toegevoegd en begin gemaakt aan de code</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +489,9 @@
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -496,18 +504,24 @@
         <f t="shared" si="0"/>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>0.46875</v>
+      </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>-0.39583333333333331</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>7.2916666666666685E-2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -592,7 +606,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>-0.23958333333333326</v>
+        <v>0.22916666666666674</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -760,7 +774,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,25 +825,35 @@
         <f t="shared" si="0"/>
         <v>0.10416666666666674</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>0.46875</v>
+      </c>
       <c r="C4" s="3">
         <f t="shared" si="0"/>
-        <v>-0.39583333333333331</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>7.2916666666666685E-2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="3">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11458333333333326</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -916,7 +940,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>-0.22916666666666657</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Changed some code, and pre-added excel time
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08cc52190196310d/Documenten/TBA/Non-Code Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karsten Keemink\Desktop\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{7916A1DC-09DC-4251-B336-81ECA4145E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C8BCE8-4BF3-4970-9294-8A0ADC49239E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9248B92-BC02-4A1C-B254-D0F2C7E29DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
     <sheet name="Douwe" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -51,6 +53,12 @@
   </si>
   <si>
     <t>Laatste voorlogie locatie toegevoegd en begin gemaakt aan de code</t>
+  </si>
+  <si>
+    <t>Douwe's code bekeken en in apart vsC bestand gekeken of het beter kon</t>
+  </si>
+  <si>
+    <t>Verschillende defs en commands aangepast voor performance en Ease of Use</t>
   </si>
 </sst>
 </file>
@@ -132,7 +140,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,19 +445,19 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -463,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -478,7 +486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.60416666666666663</v>
       </c>
@@ -493,7 +501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.65625</v>
       </c>
@@ -508,7 +516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.39583333333333331</v>
       </c>
@@ -523,25 +531,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.625</v>
+      </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -550,7 +570,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -559,7 +579,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -568,7 +588,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -577,7 +597,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -586,7 +606,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -595,166 +615,166 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>0.22916666666666674</v>
+        <v>0.38194444444444442</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -773,19 +793,19 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -799,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.4375</v>
       </c>
@@ -814,7 +834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.60416666666666663</v>
       </c>
@@ -829,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.39583333333333331</v>
       </c>
@@ -844,7 +864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.55208333333333337</v>
       </c>
@@ -857,7 +877,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -866,7 +886,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -875,7 +895,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -884,7 +904,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -893,7 +913,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -902,7 +922,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -911,7 +931,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -920,7 +940,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -929,13 +949,13 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5">
@@ -944,151 +964,151 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>

</xml_diff>

<commit_message>
changed colors and stuff, also added days to excel
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karsten Keemink\Desktop\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9248B92-BC02-4A1C-B254-D0F2C7E29DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5623EB60-F463-4F13-8811-28192EBC8A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>Verschillende defs en commands aangepast voor performance en Ease of Use</t>
+  </si>
+  <si>
+    <t>Dag</t>
+  </si>
+  <si>
+    <t>Maandag</t>
+  </si>
+  <si>
+    <t>dinsdag</t>
+  </si>
+  <si>
+    <t>woensdag</t>
   </si>
 </sst>
 </file>
@@ -443,10 +455,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,9 +467,10 @@
     <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="100.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -470,8 +483,11 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -485,8 +501,11 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.60416666666666663</v>
       </c>
@@ -501,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.65625</v>
       </c>
@@ -516,7 +535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.39583333333333331</v>
       </c>
@@ -530,8 +549,11 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.57638888888888895</v>
       </c>
@@ -546,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0.4375</v>
       </c>
@@ -560,8 +582,11 @@
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -570,7 +595,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -579,7 +604,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -588,7 +613,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -597,7 +622,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -606,7 +631,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -615,13 +640,13 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5">
@@ -630,7 +655,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -791,10 +816,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +830,7 @@
     <col min="4" max="4" width="100.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -818,8 +843,11 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.4375</v>
       </c>
@@ -833,8 +861,11 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.60416666666666663</v>
       </c>
@@ -849,7 +880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.39583333333333331</v>
       </c>
@@ -863,8 +894,11 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.55208333333333337</v>
       </c>
@@ -877,7 +911,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
@@ -885,8 +919,11 @@
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -895,7 +932,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -904,7 +941,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -913,7 +950,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -922,7 +959,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -931,7 +968,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -940,7 +977,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -949,13 +986,13 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5">
@@ -964,7 +1001,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
mijn tijden in logboek gezet
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karsten Keemink\Desktop\TBA\Non-Code Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB08DBB7-D76E-42C0-A554-E5CA37B22BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86813385-0780-4CFD-8DA4-F73A190332BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
     <sheet name="Douwe" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -71,6 +69,12 @@
   </si>
   <si>
     <t>Verschillende defs en commands aangepast voor performance en Ease of Use + json aangepast</t>
+  </si>
+  <si>
+    <t>Verder gewerkt aan de code van de eerste kamer</t>
+  </si>
+  <si>
+    <t>Begin gemaakt aan de derde ruimte van onze game. Ook gewerkt aan de geheime ruimte</t>
   </si>
 </sst>
 </file>
@@ -152,7 +156,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,7 +461,7 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -818,8 +822,8 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,16 +913,24 @@
         <f t="shared" si="0"/>
         <v>0.11458333333333326</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.5625</v>
+      </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
@@ -997,7 +1009,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>0.35416666666666669</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Karsten zijn tijd ingevoerd
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B23285-510A-40AC-BF40-641F467CE658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C641F81D-51A3-46D7-ADDD-F2580F5AE6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Verder gewerkt aan kamer 3 en geheime kamer, ook aan een functie gezeten om items te equippen</t>
+  </si>
+  <si>
+    <t>In apart bestand kamers uitgewerkt dat ik moet coderen</t>
   </si>
 </sst>
 </file>
@@ -464,8 +467,8 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +607,9 @@
         <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -829,7 +834,7 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ruimte 5 met subruimtes is af. ook heb ik de equip een beetje anders gedaan.
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBA\Non-Code Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08cc52190196310d/Documenten/TBA/Non-Code Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C641F81D-51A3-46D7-ADDD-F2580F5AE6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C641F81D-51A3-46D7-ADDD-F2580F5AE6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4B0E987-BEF0-4D03-988C-5D10103F0C0E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
@@ -467,20 +467,20 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0.60416666666666663</v>
       </c>
@@ -530,7 +530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0.65625</v>
       </c>
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.39583333333333331</v>
       </c>
@@ -563,7 +563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0.57638888888888895</v>
       </c>
@@ -578,7 +578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0.4375</v>
       </c>
@@ -596,7 +596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0.58333333333333337</v>
       </c>
@@ -611,7 +611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -620,7 +620,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -629,7 +629,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -638,7 +638,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -647,7 +647,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -656,13 +656,13 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5">
@@ -671,151 +671,151 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -834,19 +834,19 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.44140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -863,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0.4375</v>
       </c>
@@ -881,7 +881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0.60416666666666663</v>
       </c>
@@ -896,7 +896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0.39583333333333331</v>
       </c>
@@ -914,7 +914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.55208333333333337</v>
       </c>
@@ -929,7 +929,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0.4375</v>
       </c>
@@ -947,7 +947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0.58333333333333337</v>
       </c>
@@ -962,16 +962,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11458333333333331</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -980,16 +984,15 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -998,7 +1001,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -1007,7 +1010,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -1016,166 +1019,166 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>0.64583333333333326</v>
+        <v>0.76041666666666652</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>

</xml_diff>

<commit_message>
ik haat git merge conflicts
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBA\Non-Code Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karsten Keemink\Desktop\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA06D79-4E5E-40A5-9A87-5F5E52680360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA06752C-915A-44AA-9D2F-0D560E50929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
     <sheet name="Douwe" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -177,7 +179,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>

</xml_diff>

<commit_message>
logboek voor vandaag aangepast
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karsten Keemink\Desktop\TBA\Non-Code Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA06752C-915A-44AA-9D2F-0D560E50929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1462CB-F33F-43D8-8898-723614D9A29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
     <sheet name="Douwe" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -97,7 +95,15 @@
     <t>vrijdag</t>
   </si>
   <si>
-    <t>Functie gemaakt om eten te kunnen eten en een idee uitgewerkt voor ruimte 9</t>
+    <t>Functie gemaakt om eten te kunnen eten en begonnen met het maken van ruimte 9</t>
+  </si>
+  <si>
+    <t>Op papier eerst een ''snakes and ladders'' ascii art gemaakt om het vervolgens in python uit te printen. 
+Het is voor een klimpuzzel in ruimte 9
+Op deze website is het gedaan https://asciiflow.com/#/</t>
+  </si>
+  <si>
+    <t>zaterdag</t>
   </si>
 </sst>
 </file>
@@ -157,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,9 +183,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -852,7 +861,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,14 +1040,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -1048,6 +1063,9 @@
         <v>0</v>
       </c>
       <c r="D12" s="1"/>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -1069,7 +1087,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>1.0104166666666665</v>
+        <v>1.0729166666666665</v>
       </c>
       <c r="D15" s="1"/>
     </row>

</xml_diff>

<commit_message>
comments geschreven bij code en logboek verbterd
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF32AB4-BA18-4892-903B-1C16EA424C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0238F93D-0BB9-495C-AD82-1531593DE9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>donderdag</t>
-  </si>
-  <si>
-    <t>Gewerkt aan kamer 7, ook wel het ravijn genoemd.</t>
   </si>
   <si>
     <t>Kamer 5 met alle subrooms afgekregen, ook wel het dorp, en de equip functie verbeterd</t>
@@ -107,6 +104,19 @@
   </si>
   <si>
     <t>De klimpuzzel helemaal gecodeerd, alleen nog een geheimer ruimte nodig op Plek H</t>
+  </si>
+  <si>
+    <t>Zondag</t>
+  </si>
+  <si>
+    <t>Besloten om bij plek H toch niet een hele ruimte te maken.
+En Vervolgens besloten om de code door te lezen en te verbeteren.
+Ook ervoor gezorgd dat er een paar comments door de code heen staan om het uit te leggen.</t>
+  </si>
+  <si>
+    <t>Gewerkt aan kamer 7, ook wel het ravijn genoemd.
+Ook de puzzel geluid af laten spelen met playsound.
+De puzzel is het oplossen van Morse Code.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,7 +197,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,7 +880,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +920,7 @@
         <f t="shared" ref="C2:C13" si="0">B2-A2</f>
         <v>6.25E-2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
@@ -922,7 +938,7 @@
         <f t="shared" si="0"/>
         <v>0.10416666666666674</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -937,7 +953,7 @@
         <f t="shared" si="0"/>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
@@ -955,7 +971,7 @@
         <f t="shared" si="0"/>
         <v>0.11458333333333326</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -970,7 +986,7 @@
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E6" t="s">
@@ -988,7 +1004,7 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1003,14 +1019,14 @@
         <f t="shared" si="0"/>
         <v>0.11458333333333331</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
+      <c r="D8" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -1021,8 +1037,8 @@
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
+      <c r="D9" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1036,11 +1052,11 @@
         <f t="shared" si="0"/>
         <v>0.12499999999999994</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
+      <c r="D10" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1054,8 +1070,8 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
+      <c r="D11" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,27 +1079,36 @@
         <v>0.5625</v>
       </c>
       <c r="B12" s="3">
-        <v>0.60416666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="D12" s="1" t="s">
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1096,7 +1121,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="5">
         <f>SUM(C2:C14)</f>
-        <v>1.114583333333333</v>
+        <v>1.1979166666666667</v>
       </c>
       <c r="D15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added dissapeared rooms back and coded more functions
Co-authored-by: Douwe Zumker <Peredurz@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TBA\Non-Code Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karsten Keemink\Desktop\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0238F93D-0BB9-495C-AD82-1531593DE9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0B18BD-9821-4ECF-9EB8-1589F7CF983B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karsten" sheetId="1" r:id="rId1"/>
     <sheet name="Douwe" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -117,6 +119,30 @@
     <t>Gewerkt aan kamer 7, ook wel het ravijn genoemd.
 Ook de puzzel geluid af laten spelen met playsound.
 De puzzel is het oplossen van Morse Code.</t>
+  </si>
+  <si>
+    <t>Room 4 en 6 gemaakt</t>
+  </si>
+  <si>
+    <t>room 6  en subrooms afgemaakt begonnen aan room 8</t>
+  </si>
+  <si>
+    <t>room 8 en subrooms afgemaakt en gepushed naar git (MERGE CONFLICT)</t>
+  </si>
+  <si>
+    <t>Code verbeterd en voor de rest niet veel gedaan(uit eten met familie)</t>
+  </si>
+  <si>
+    <t>zondag</t>
+  </si>
+  <si>
+    <t>maandag</t>
+  </si>
+  <si>
+    <t>Die merge conflict had mijn progress verwijdert en Douwe's files overgekopieerd Room 4, 6 en 8 waren weg. Room 4 6 en 8 opnieuw gemaakt en begonnen room 10</t>
+  </si>
+  <si>
+    <t>Meerdere nieuwe functies aangemaakt en code performance wise aangepast voor minder opgeslagen cache etc (niet while loops pauzeren en andere dingen doen maar echt afsluiten)</t>
   </si>
 </sst>
 </file>
@@ -207,7 +233,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,10 +536,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +547,7 @@
     <col min="1" max="1" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="149.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -550,7 +576,7 @@
         <v>0.5</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C13" si="0">B2-A2</f>
+        <f t="shared" ref="C2:C15" si="0">B2-A2</f>
         <v>8.3333333333333315E-2</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -657,69 +683,122 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>0.22916666666666663</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+        <v>6.2499999999999944E-2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.21527777777777773</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5">
-        <f>SUM(C2:C14)</f>
-        <v>0.56944444444444442</v>
-      </c>
-      <c r="D15" s="1"/>
+      <c r="A15" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.15972222222222227</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="5">
+        <f>SUM(C2:C15)</f>
+        <v>1.4236111111111109</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,6 +944,12 @@
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -879,7 +964,7 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added room 4 and 10 + subrooms, also bossfight and extra book
</commit_message>
<xml_diff>
--- a/Non-Code Files/Logboek.xlsx
+++ b/Non-Code Files/Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karsten Keemink\Desktop\TBA\Non-Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3229B-7E33-49CF-B0AB-2EB800786378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B967F0E-4A29-490D-8B66-F8B69256014E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Begin Tijd</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Karsten geholpen met nieuwe functies bouwen en het hercoderen van de "verdwenen" Rooms, ook nog extra verhaal toegevoegd</t>
+  </si>
+  <si>
+    <t>Room 10 en 4 afgemaakt inclusief subrooms. Ook boss fight gemaakt en puzzel toegevoegd. Dinsdag laatste hand aan room8</t>
   </si>
 </sst>
 </file>
@@ -539,10 +542,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +553,7 @@
     <col min="1" max="1" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="149.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="168.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -579,7 +582,7 @@
         <v>0.5</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C15" si="0">B2-A2</f>
+        <f t="shared" ref="C2:C16" si="0">B2-A2</f>
         <v>8.3333333333333315E-2</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -780,41 +783,49 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="C15" s="3">
+        <f>B15-A15</f>
+        <v>0.25694444444444431</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>0.61805555555555558</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="3">
         <f t="shared" si="0"/>
         <v>0.15972222222222227</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="5">
-        <f>SUM(C2:C15)</f>
-        <v>1.4236111111111109</v>
-      </c>
-      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="5">
+        <f>SUM(C2:C16)</f>
+        <v>1.6805555555555554</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -953,6 +964,12 @@
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -965,10 +982,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1022,7 @@
         <v>0.5</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C14" si="0">B2-A2</f>
+        <f>B2-A2</f>
         <v>6.25E-2</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -1023,7 +1040,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" si="0"/>
+        <f>B3-A3</f>
         <v>0.10416666666666674</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1038,7 +1055,7 @@
         <v>0.46875</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
+        <f>B4-A4</f>
         <v>7.2916666666666685E-2</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -1056,7 +1073,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="0"/>
+        <f>B5-A5</f>
         <v>0.11458333333333326</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1071,7 +1088,7 @@
         <v>0.5625</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
+        <f>B6-A6</f>
         <v>0.125</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1089,7 +1106,7 @@
         <v>0.75</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
+        <f>B7-A7</f>
         <v>0.16666666666666663</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1104,7 +1121,7 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
+        <f>B8-A8</f>
         <v>0.11458333333333331</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1122,7 +1139,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
+        <f>B9-A9</f>
         <v>0.125</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -1137,7 +1154,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="0"/>
+        <f>B10-A10</f>
         <v>0.12499999999999994</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -1155,7 +1172,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="0"/>
+        <f>B11-A11</f>
         <v>6.25E-2</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -1170,7 +1187,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="0"/>
+        <f>B12-A12</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -1188,7 +1205,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="0"/>
+        <f>B13-A13</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1198,7 +1215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0.52777777777777779</v>
       </c>
@@ -1206,7 +1223,7 @@
         <v>0.6875</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="0"/>
+        <f>B14-A14</f>
         <v>0.15972222222222221</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1216,25 +1233,20 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5">
-        <f>SUM(C2:C14)</f>
-        <v>1.3576388888888888</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C2:C14)</f>
+        <v>1.3576388888888888</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1375,6 +1387,12 @@
       <c r="C40" s="3"/>
       <c r="D40" s="1"/>
     </row>
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>